<commit_message>
little changes to file download
</commit_message>
<xml_diff>
--- a/client/public/pyreport/report3.xlsx
+++ b/client/public/pyreport/report3.xlsx
@@ -4620,33 +4620,15 @@
         </is>
       </c>
       <c r="F14" s="91" t="n"/>
-      <c r="G14" s="41" t="n">
-        <v/>
-      </c>
-      <c r="H14" s="42" t="n">
-        <v/>
-      </c>
-      <c r="I14" s="43" t="n">
-        <v/>
-      </c>
-      <c r="J14" s="41" t="n">
-        <v/>
-      </c>
-      <c r="K14" s="42" t="n">
-        <v/>
-      </c>
-      <c r="L14" s="43" t="n">
-        <v/>
-      </c>
-      <c r="M14" s="41" t="n">
-        <v/>
-      </c>
-      <c r="N14" s="42" t="n">
-        <v/>
-      </c>
-      <c r="O14" s="43" t="n">
-        <v/>
-      </c>
+      <c r="G14" s="41" t="n"/>
+      <c r="H14" s="42" t="n"/>
+      <c r="I14" s="43" t="n"/>
+      <c r="J14" s="41" t="n"/>
+      <c r="K14" s="42" t="n"/>
+      <c r="L14" s="43" t="n"/>
+      <c r="M14" s="41" t="n"/>
+      <c r="N14" s="42" t="n"/>
+      <c r="O14" s="43" t="n"/>
       <c r="P14" s="92" t="n">
         <v>41.1</v>
       </c>
@@ -4672,33 +4654,15 @@
         </is>
       </c>
       <c r="F15" s="91" t="n"/>
-      <c r="G15" s="44" t="n">
-        <v/>
-      </c>
-      <c r="H15" s="42" t="n">
-        <v/>
-      </c>
-      <c r="I15" s="45" t="n">
-        <v/>
-      </c>
-      <c r="J15" s="44" t="n">
-        <v/>
-      </c>
-      <c r="K15" s="42" t="n">
-        <v/>
-      </c>
-      <c r="L15" s="45" t="n">
-        <v/>
-      </c>
-      <c r="M15" s="44" t="n">
-        <v/>
-      </c>
-      <c r="N15" s="42" t="n">
-        <v/>
-      </c>
-      <c r="O15" s="45" t="n">
-        <v/>
-      </c>
+      <c r="G15" s="44" t="n"/>
+      <c r="H15" s="42" t="n"/>
+      <c r="I15" s="45" t="n"/>
+      <c r="J15" s="44" t="n"/>
+      <c r="K15" s="42" t="n"/>
+      <c r="L15" s="45" t="n"/>
+      <c r="M15" s="44" t="n"/>
+      <c r="N15" s="42" t="n"/>
+      <c r="O15" s="45" t="n"/>
       <c r="P15" s="92" t="n">
         <v>20.6</v>
       </c>
@@ -7559,7 +7523,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing SILT-TRAP new piezometer
</commit_message>
<xml_diff>
--- a/client/public/pyreport/report3.xlsx
+++ b/client/public/pyreport/report3.xlsx
@@ -4344,7 +4344,7 @@
       </c>
       <c r="L5" s="8" t="n"/>
       <c r="M5" s="69" t="n">
-        <v>45119</v>
+        <v>45120</v>
       </c>
       <c r="N5" s="81" t="n"/>
       <c r="O5" s="81" t="n"/>
@@ -4695,7 +4695,7 @@
         <v>86.74505000000001</v>
       </c>
       <c r="I16" s="45" t="n">
-        <v>86.39066788372094</v>
+        <v>86.3906925</v>
       </c>
       <c r="J16" s="44" t="n">
         <v>85.988609</v>
@@ -4704,7 +4704,7 @@
         <v>86.933869</v>
       </c>
       <c r="L16" s="45" t="n">
-        <v>86.42015858333333</v>
+        <v>86.41385455</v>
       </c>
       <c r="M16" s="44" t="n">
         <v>85.988609</v>
@@ -4713,7 +4713,7 @@
         <v>88.06814900000001</v>
       </c>
       <c r="O16" s="45" t="n">
-        <v>86.9689452354049</v>
+        <v>86.95434500564971</v>
       </c>
       <c r="P16" s="92" t="n">
         <v>27</v>
@@ -4747,7 +4747,7 @@
         <v>-19.756494</v>
       </c>
       <c r="I17" s="45" t="n">
-        <v>-20.14269943548387</v>
+        <v>-20.147213078125</v>
       </c>
       <c r="J17" s="44" t="n">
         <v>-20.625188</v>
@@ -4756,7 +4756,7 @@
         <v>-19.756494</v>
       </c>
       <c r="L17" s="45" t="n">
-        <v>-20.25479981818182</v>
+        <v>-20.25391708275862</v>
       </c>
       <c r="M17" s="44" t="n">
         <v>-21.011479</v>
@@ -4765,7 +4765,7 @@
         <v>-19.756494</v>
       </c>
       <c r="O17" s="45" t="n">
-        <v>-20.42842572134832</v>
+        <v>-20.42237500896861</v>
       </c>
       <c r="P17" s="92" t="n">
         <v>25.5</v>
@@ -4799,7 +4799,7 @@
         <v>-8.025601</v>
       </c>
       <c r="I18" s="45" t="n">
-        <v>-8.109691225806452</v>
+        <v>-8.111200484375001</v>
       </c>
       <c r="J18" s="44" t="n">
         <v>-8.289662</v>
@@ -4808,7 +4808,7 @@
         <v>-7.762332</v>
       </c>
       <c r="L18" s="45" t="n">
-        <v>-8.027150965034965</v>
+        <v>-8.035023441379311</v>
       </c>
       <c r="M18" s="44" t="n">
         <v>-8.289662</v>
@@ -4817,7 +4817,7 @@
         <v>-7.322865</v>
       </c>
       <c r="O18" s="45" t="n">
-        <v>-7.807787316853933</v>
+        <v>-7.815965899103139</v>
       </c>
       <c r="P18" s="92" t="n">
         <v>28.2</v>
@@ -4851,7 +4851,7 @@
         <v>37.306932</v>
       </c>
       <c r="I19" s="45" t="n">
-        <v>37.13815053424658</v>
+        <v>37.13733622368421</v>
       </c>
       <c r="J19" s="44" t="n">
         <v>36.927846</v>
@@ -4860,7 +4860,7 @@
         <v>37.307008</v>
       </c>
       <c r="L19" s="45" t="n">
-        <v>37.16960696153846</v>
+        <v>37.16624002515723</v>
       </c>
       <c r="M19" s="44" t="n">
         <v>36.927846</v>
@@ -4869,7 +4869,7 @@
         <v>38.066237</v>
       </c>
       <c r="O19" s="45" t="n">
-        <v>37.40713528444444</v>
+        <v>37.39849464301552</v>
       </c>
       <c r="P19" s="92" t="n">
         <v>42</v>
@@ -4903,7 +4903,7 @@
         <v>31.397185</v>
       </c>
       <c r="I20" s="45" t="n">
-        <v>31.06757755072464</v>
+        <v>31.06506166666667</v>
       </c>
       <c r="J20" s="44" t="n">
         <v>30.702711</v>
@@ -4912,16 +4912,16 @@
         <v>31.397208</v>
       </c>
       <c r="L20" s="45" t="n">
-        <v>31.05691536666667</v>
+        <v>31.05112804666667</v>
       </c>
       <c r="M20" s="44" t="n">
         <v>30.702711</v>
       </c>
       <c r="N20" s="42" t="n">
-        <v>31.745893</v>
+        <v>31.572313</v>
       </c>
       <c r="O20" s="45" t="n">
-        <v>31.16210617505471</v>
+        <v>31.15830040919037</v>
       </c>
       <c r="P20" s="92" t="n">
         <v>18.3</v>
@@ -4955,16 +4955,16 @@
         <v>39.829119</v>
       </c>
       <c r="I21" s="45" t="n">
-        <v>39.2571523125</v>
+        <v>39.25920927710843</v>
       </c>
       <c r="J21" s="44" t="n">
         <v>37.91027</v>
       </c>
       <c r="K21" s="42" t="n">
-        <v>39.832252</v>
+        <v>39.831167</v>
       </c>
       <c r="L21" s="45" t="n">
-        <v>39.0392672</v>
+        <v>39.02679032934132</v>
       </c>
       <c r="M21" s="44" t="n">
         <v>37.720579</v>
@@ -4973,7 +4973,7 @@
         <v>39.832263</v>
       </c>
       <c r="O21" s="45" t="n">
-        <v>38.74643455911824</v>
+        <v>38.75746613426854</v>
       </c>
       <c r="P21" s="92" t="n">
         <v>9.300000000000001</v>
@@ -5007,7 +5007,7 @@
         <v>88.11657</v>
       </c>
       <c r="I22" s="45" t="n">
-        <v>87.81584141935484</v>
+        <v>87.816848515625</v>
       </c>
       <c r="J22" s="44" t="n">
         <v>87.398082</v>
@@ -5016,7 +5016,7 @@
         <v>88.11657</v>
       </c>
       <c r="L22" s="45" t="n">
-        <v>87.77338716901409</v>
+        <v>87.77348341134751</v>
       </c>
       <c r="M22" s="44" t="n">
         <v>87.398082</v>
@@ -5025,7 +5025,7 @@
         <v>88.117524</v>
       </c>
       <c r="O22" s="45" t="n">
-        <v>87.78579072911964</v>
+        <v>87.78543723303167</v>
       </c>
       <c r="P22" s="92" t="n">
         <v>14.3</v>
@@ -5053,13 +5053,13 @@
       </c>
       <c r="F23" s="91" t="n"/>
       <c r="G23" s="44" t="n">
-        <v>-5.265736</v>
+        <v>-5.266335</v>
       </c>
       <c r="H23" s="42" t="n">
         <v>-4.710974</v>
       </c>
       <c r="I23" s="45" t="n">
-        <v>-4.974705309523809</v>
+        <v>-4.981120731707317</v>
       </c>
       <c r="J23" s="44" t="n">
         <v>-5.544583</v>
@@ -5068,7 +5068,7 @@
         <v>-4.710974</v>
       </c>
       <c r="L23" s="45" t="n">
-        <v>-5.095856887755102</v>
+        <v>-5.1009746875</v>
       </c>
       <c r="M23" s="44" t="n">
         <v>-5.823333</v>
@@ -5077,7 +5077,7 @@
         <v>-4.710974</v>
       </c>
       <c r="O23" s="45" t="n">
-        <v>-5.26581983203125</v>
+        <v>-5.26309591015625</v>
       </c>
       <c r="P23" s="92" t="n">
         <v>23.5</v>
@@ -5111,7 +5111,7 @@
         <v>-2.983156</v>
       </c>
       <c r="I24" s="45" t="n">
-        <v>-3.291722976190476</v>
+        <v>-3.289214463414634</v>
       </c>
       <c r="J24" s="44" t="n">
         <v>-3.803501</v>
@@ -5120,7 +5120,7 @@
         <v>-2.983156</v>
       </c>
       <c r="L24" s="45" t="n">
-        <v>-3.412685081632653</v>
+        <v>-3.41163653125</v>
       </c>
       <c r="M24" s="44" t="n">
         <v>-4.35267</v>
@@ -5129,7 +5129,7 @@
         <v>-2.983156</v>
       </c>
       <c r="O24" s="45" t="n">
-        <v>-3.598204953125</v>
+        <v>-3.59338476953125</v>
       </c>
       <c r="P24" s="92" t="n">
         <v>26</v>
@@ -5160,19 +5160,19 @@
         <v>-23.20302</v>
       </c>
       <c r="H25" s="42" t="n">
-        <v>-22.639895</v>
+        <v>-22.826769</v>
       </c>
       <c r="I25" s="45" t="n">
-        <v>-23.0274335409836</v>
+        <v>-23.03935558064516</v>
       </c>
       <c r="J25" s="44" t="n">
         <v>-23.390645</v>
       </c>
       <c r="K25" s="42" t="n">
-        <v>-22.639203</v>
+        <v>-22.639895</v>
       </c>
       <c r="L25" s="45" t="n">
-        <v>-23.06749979452055</v>
+        <v>-23.07695473103448</v>
       </c>
       <c r="M25" s="44" t="n">
         <v>-23.390645</v>
@@ -5181,7 +5181,7 @@
         <v>-22.44753</v>
       </c>
       <c r="O25" s="45" t="n">
-        <v>-22.95641968874172</v>
+        <v>-22.95994596895787</v>
       </c>
       <c r="P25" s="92" t="n">
         <v>11</v>
@@ -5215,7 +5215,7 @@
         <v>62.482372</v>
       </c>
       <c r="I26" s="45" t="n">
-        <v>62.223971609375</v>
+        <v>62.22038748484849</v>
       </c>
       <c r="J26" s="44" t="n">
         <v>62.105822</v>
@@ -5224,16 +5224,16 @@
         <v>62.66958</v>
       </c>
       <c r="L26" s="45" t="n">
-        <v>62.27106623448276</v>
+        <v>62.26069517241379</v>
       </c>
       <c r="M26" s="44" t="n">
         <v>62.105822</v>
       </c>
       <c r="N26" s="42" t="n">
-        <v>63.607747</v>
+        <v>63.420533</v>
       </c>
       <c r="O26" s="45" t="n">
-        <v>62.57375029464286</v>
+        <v>62.55908508258928</v>
       </c>
       <c r="P26" s="92" t="n">
         <v>42</v>
@@ -5267,7 +5267,7 @@
         <v>-22.616509</v>
       </c>
       <c r="I27" s="45" t="n">
-        <v>-22.88745868421053</v>
+        <v>-22.89351830769231</v>
       </c>
       <c r="J27" s="44" t="n">
         <v>-23.317784</v>
@@ -5276,7 +5276,7 @@
         <v>-22.616509</v>
       </c>
       <c r="L27" s="45" t="n">
-        <v>-22.98781310625</v>
+        <v>-22.99053644654088</v>
       </c>
       <c r="M27" s="44" t="n">
         <v>-23.645557</v>
@@ -5285,7 +5285,7 @@
         <v>-22.616509</v>
       </c>
       <c r="O27" s="45" t="n">
-        <v>-23.13550264102564</v>
+        <v>-23.13243188167053</v>
       </c>
       <c r="P27" s="92" t="n">
         <v>20</v>
@@ -5319,7 +5319,7 @@
         <v>-23.091399</v>
       </c>
       <c r="I28" s="45" t="n">
-        <v>-23.34697988157895</v>
+        <v>-23.34305237179487</v>
       </c>
       <c r="J28" s="44" t="n">
         <v>-23.696599</v>
@@ -5328,7 +5328,7 @@
         <v>-23.091399</v>
       </c>
       <c r="L28" s="45" t="n">
-        <v>-23.4428257</v>
+        <v>-23.4414237672956</v>
       </c>
       <c r="M28" s="44" t="n">
         <v>-24.062188</v>
@@ -5337,7 +5337,7 @@
         <v>-23.091399</v>
       </c>
       <c r="O28" s="45" t="n">
-        <v>-23.61542446153846</v>
+        <v>-23.61091456148492</v>
       </c>
       <c r="P28" s="92" t="n">
         <v>23.2</v>
@@ -5371,7 +5371,7 @@
         <v>-20.721999</v>
       </c>
       <c r="I29" s="45" t="n">
-        <v>-20.97798664473684</v>
+        <v>-20.97873274358975</v>
       </c>
       <c r="J29" s="44" t="n">
         <v>-21.368161</v>
@@ -5380,7 +5380,7 @@
         <v>-20.721999</v>
       </c>
       <c r="L29" s="45" t="n">
-        <v>-21.07231865625</v>
+        <v>-21.07253074842767</v>
       </c>
       <c r="M29" s="44" t="n">
         <v>-21.616989</v>
@@ -5389,7 +5389,7 @@
         <v>-20.721999</v>
       </c>
       <c r="O29" s="45" t="n">
-        <v>-21.21458081818182</v>
+        <v>-21.21104851740139</v>
       </c>
       <c r="P29" s="92" t="n">
         <v>24.4</v>
@@ -5423,7 +5423,7 @@
         <v>-22.273053</v>
       </c>
       <c r="I30" s="45" t="n">
-        <v>-22.53012661251863</v>
+        <v>-22.52652623363095</v>
       </c>
       <c r="J30" s="44" t="n">
         <v>-22.96156</v>
@@ -5432,7 +5432,7 @@
         <v>-22.273053</v>
       </c>
       <c r="L30" s="45" t="n">
-        <v>-22.64008125621008</v>
+        <v>-22.6364553787234</v>
       </c>
       <c r="M30" s="44" t="n">
         <v>-23.229077</v>
@@ -5441,7 +5441,7 @@
         <v>-22.273053</v>
       </c>
       <c r="O30" s="45" t="n">
-        <v>-22.81079990351299</v>
+        <v>-22.80554812698413</v>
       </c>
       <c r="P30" s="92" t="n">
         <v>24</v>
@@ -5469,22 +5469,22 @@
       </c>
       <c r="F31" s="91" t="n"/>
       <c r="G31" s="44" t="n">
-        <v>9.021815</v>
+        <v>9.021986999999999</v>
       </c>
       <c r="H31" s="42" t="n">
         <v>9.900392</v>
       </c>
       <c r="I31" s="45" t="n">
-        <v>9.393308157894737</v>
+        <v>9.441071786666667</v>
       </c>
       <c r="J31" s="44" t="n">
-        <v>8.147027</v>
+        <v>8.290679000000001</v>
       </c>
       <c r="K31" s="42" t="n">
         <v>9.900392</v>
       </c>
       <c r="L31" s="45" t="n">
-        <v>9.01853517791411</v>
+        <v>9.060924765432098</v>
       </c>
       <c r="M31" s="44" t="n">
         <v>8.145104999999999</v>
@@ -5493,7 +5493,7 @@
         <v>10.045468</v>
       </c>
       <c r="O31" s="45" t="n">
-        <v>9.257058634538152</v>
+        <v>9.263599467741935</v>
       </c>
       <c r="P31" s="92" t="n">
         <v>30</v>
@@ -5527,7 +5527,7 @@
         <v>-5.724124</v>
       </c>
       <c r="I32" s="45" t="n">
-        <v>-6.058838453488372</v>
+        <v>-6.057166639534883</v>
       </c>
       <c r="J32" s="44" t="n">
         <v>-6.55158</v>
@@ -5536,7 +5536,7 @@
         <v>-5.724124</v>
       </c>
       <c r="L32" s="45" t="n">
-        <v>-6.170073840909091</v>
+        <v>-6.166863142045455</v>
       </c>
       <c r="M32" s="44" t="n">
         <v>-6.969441</v>
@@ -5545,7 +5545,7 @@
         <v>-5.724124</v>
       </c>
       <c r="O32" s="45" t="n">
-        <v>-6.374857848425197</v>
+        <v>-6.368013773622047</v>
       </c>
       <c r="P32" s="92" t="n">
         <v>16</v>
@@ -5579,7 +5579,7 @@
         <v>28.982453</v>
       </c>
       <c r="I33" s="45" t="n">
-        <v>27.52976510526316</v>
+        <v>27.68073685897436</v>
       </c>
       <c r="J33" s="44" t="n">
         <v>24.075044</v>
@@ -5588,7 +5588,7 @@
         <v>28.982453</v>
       </c>
       <c r="L33" s="45" t="n">
-        <v>26.32932577070064</v>
+        <v>26.41896805063291</v>
       </c>
       <c r="M33" s="44" t="n">
         <v>24.075044</v>
@@ -5597,7 +5597,7 @@
         <v>28.982453</v>
       </c>
       <c r="O33" s="45" t="n">
-        <v>25.80733416557734</v>
+        <v>25.83185688043478</v>
       </c>
       <c r="P33" s="92" t="n">
         <v>15</v>
@@ -5625,13 +5625,13 @@
       </c>
       <c r="F34" s="91" t="n"/>
       <c r="G34" s="44" t="n">
-        <v>-6.719582</v>
+        <v>-6.711448</v>
       </c>
       <c r="H34" s="42" t="n">
         <v>-6.366213</v>
       </c>
       <c r="I34" s="45" t="n">
-        <v>-6.569952327407408</v>
+        <v>-6.558387199409158</v>
       </c>
       <c r="J34" s="44" t="n">
         <v>-7.011278</v>
@@ -5640,16 +5640,16 @@
         <v>-6.366213</v>
       </c>
       <c r="L34" s="45" t="n">
-        <v>-6.649185882656827</v>
+        <v>-6.638929148609078</v>
       </c>
       <c r="M34" s="44" t="n">
-        <v>-7.456504</v>
+        <v>-7.455692</v>
       </c>
       <c r="N34" s="42" t="n">
         <v>-6.366213</v>
       </c>
       <c r="O34" s="45" t="n">
-        <v>-6.92088312608486</v>
+        <v>-6.912456613603474</v>
       </c>
       <c r="P34" s="92" t="n">
         <v>2</v>
@@ -5677,13 +5677,13 @@
       </c>
       <c r="F35" s="91" t="n"/>
       <c r="G35" s="44" t="n">
-        <v>45.424404</v>
+        <v>45.424535</v>
       </c>
       <c r="H35" s="42" t="n">
         <v>46.194645</v>
       </c>
       <c r="I35" s="45" t="n">
-        <v>45.69019255405406</v>
+        <v>45.6973764025974</v>
       </c>
       <c r="J35" s="44" t="n">
         <v>45.424404</v>
@@ -5692,7 +5692,7 @@
         <v>46.194645</v>
       </c>
       <c r="L35" s="45" t="n">
-        <v>45.71371409027778</v>
+        <v>45.71105320547945</v>
       </c>
       <c r="M35" s="44" t="n">
         <v>45.233122</v>
@@ -5701,7 +5701,7 @@
         <v>46.195093</v>
       </c>
       <c r="O35" s="45" t="n">
-        <v>45.71332059277108</v>
+        <v>45.71400952403846</v>
       </c>
       <c r="P35" s="92" t="n">
         <v>30.8</v>
@@ -5735,7 +5735,7 @@
         <v>1.209078</v>
       </c>
       <c r="I36" s="45" t="n">
-        <v>1.036207811594203</v>
+        <v>1.025189328571429</v>
       </c>
       <c r="J36" s="44" t="n">
         <v>0.453479</v>
@@ -5744,7 +5744,7 @@
         <v>2.15031</v>
       </c>
       <c r="L36" s="45" t="n">
-        <v>1.226955353333333</v>
+        <v>1.210656493243243</v>
       </c>
       <c r="M36" s="44" t="n">
         <v>0.453479</v>
@@ -5753,7 +5753,7 @@
         <v>2.716051</v>
       </c>
       <c r="O36" s="45" t="n">
-        <v>1.74530386695279</v>
+        <v>1.730646819354839</v>
       </c>
       <c r="P36" s="92" t="n">
         <v>51</v>
@@ -5787,7 +5787,7 @@
         <v>53.23645</v>
       </c>
       <c r="I37" s="45" t="n">
-        <v>53.06149172463768</v>
+        <v>53.06125427142857</v>
       </c>
       <c r="J37" s="44" t="n">
         <v>52.853229</v>
@@ -5796,7 +5796,7 @@
         <v>53.429251</v>
       </c>
       <c r="L37" s="45" t="n">
-        <v>53.10745394666667</v>
+        <v>53.1005154054054</v>
       </c>
       <c r="M37" s="44" t="n">
         <v>52.853229</v>
@@ -5805,7 +5805,7 @@
         <v>54.388323</v>
       </c>
       <c r="O37" s="45" t="n">
-        <v>53.57028152575107</v>
+        <v>53.55820118494623</v>
       </c>
       <c r="P37" s="92" t="n">
         <v>69</v>
@@ -5838,7 +5838,7 @@
         <v>-19.063123</v>
       </c>
       <c r="I38" s="45" t="n">
-        <v>-19.30930202898551</v>
+        <v>-19.32201395714286</v>
       </c>
       <c r="J38" s="44" t="n">
         <v>-19.821573</v>
@@ -5847,7 +5847,7 @@
         <v>-19.063123</v>
       </c>
       <c r="L38" s="45" t="n">
-        <v>-19.40717649673203</v>
+        <v>-19.41150483006536</v>
       </c>
       <c r="M38" s="44" t="n">
         <v>-20.105456</v>
@@ -5856,7 +5856,7 @@
         <v>-19.063123</v>
       </c>
       <c r="O38" s="45" t="n">
-        <v>-19.54535894517544</v>
+        <v>-19.54286240350877</v>
       </c>
       <c r="P38" s="92" t="n">
         <v>21.3</v>
@@ -5889,7 +5889,7 @@
         <v>-18.162369</v>
       </c>
       <c r="I39" s="45" t="n">
-        <v>-18.43011146376812</v>
+        <v>-18.43431557142857</v>
       </c>
       <c r="J39" s="44" t="n">
         <v>-18.912335</v>
@@ -5898,7 +5898,7 @@
         <v>-18.162369</v>
       </c>
       <c r="L39" s="45" t="n">
-        <v>-18.50978794117647</v>
+        <v>-18.51468950326797</v>
       </c>
       <c r="M39" s="44" t="n">
         <v>-19.193832</v>
@@ -5907,7 +5907,7 @@
         <v>-18.162369</v>
       </c>
       <c r="O39" s="45" t="n">
-        <v>-18.65671445614035</v>
+        <v>-18.6532199495614</v>
       </c>
       <c r="P39" s="92" t="n">
         <v>25</v>
@@ -5939,7 +5939,7 @@
         <v>-20.583597</v>
       </c>
       <c r="I40" s="45" t="n">
-        <v>-20.91769656521739</v>
+        <v>-20.92061722857143</v>
       </c>
       <c r="J40" s="44" t="n">
         <v>-21.301471</v>
@@ -5948,7 +5948,7 @@
         <v>-20.583597</v>
       </c>
       <c r="L40" s="45" t="n">
-        <v>-21.01637836601307</v>
+        <v>-21.01755011764706</v>
       </c>
       <c r="M40" s="44" t="n">
         <v>-21.750549</v>
@@ -5957,7 +5957,7 @@
         <v>-20.583597</v>
       </c>
       <c r="O40" s="45" t="n">
-        <v>-21.15909109429824</v>
+        <v>-21.15534768201755</v>
       </c>
       <c r="P40" s="92" t="n">
         <v>26</v>
@@ -5992,7 +5992,7 @@
         <v>-19.950205</v>
       </c>
       <c r="I41" s="45" t="n">
-        <v>-23.01635052380952</v>
+        <v>-23.02049084705882</v>
       </c>
       <c r="J41" s="44" t="n">
         <v>-26.013765</v>
@@ -6001,7 +6001,7 @@
         <v>-19.950205</v>
       </c>
       <c r="L41" s="45" t="n">
-        <v>-23.04045506395349</v>
+        <v>-23.05762557803468</v>
       </c>
       <c r="M41" s="44" t="n">
         <v>-28.072206</v>
@@ -6010,7 +6010,7 @@
         <v>590.409031</v>
       </c>
       <c r="O41" s="45" t="n">
-        <v>-21.90426248033126</v>
+        <v>-21.90973085093168</v>
       </c>
       <c r="P41" s="92" t="n">
         <v>22</v>
@@ -6042,10 +6042,10 @@
         <v>-10.725058</v>
       </c>
       <c r="H42" s="42" t="n">
-        <v>-10.078292</v>
+        <v>-10.170452</v>
       </c>
       <c r="I42" s="45" t="n">
-        <v>-10.42099265217391</v>
+        <v>-10.44510925714286</v>
       </c>
       <c r="J42" s="44" t="n">
         <v>-10.725058</v>
@@ -6054,7 +6054,7 @@
         <v>-9.986136999999999</v>
       </c>
       <c r="L42" s="45" t="n">
-        <v>-10.40431129411765</v>
+        <v>-10.41878963398693</v>
       </c>
       <c r="M42" s="44" t="n">
         <v>-10.725058</v>
@@ -6063,7 +6063,7 @@
         <v>-9.524654</v>
       </c>
       <c r="O42" s="45" t="n">
-        <v>-10.16895796710526</v>
+        <v>-10.17705292763158</v>
       </c>
       <c r="P42" s="92" t="n">
         <v>28.5</v>
@@ -6092,13 +6092,13 @@
       </c>
       <c r="F43" s="91" t="n"/>
       <c r="G43" s="44" t="n">
-        <v>-22.098721</v>
+        <v>-22.098726</v>
       </c>
       <c r="H43" s="42" t="n">
         <v>-21.476649</v>
       </c>
       <c r="I43" s="45" t="n">
-        <v>-21.79606170967742</v>
+        <v>-21.802745359375</v>
       </c>
       <c r="J43" s="44" t="n">
         <v>-22.27702</v>
@@ -6107,7 +6107,7 @@
         <v>-21.476649</v>
       </c>
       <c r="L43" s="45" t="n">
-        <v>-21.90843386013986</v>
+        <v>-21.90983926896552</v>
       </c>
       <c r="M43" s="44" t="n">
         <v>-22.543371</v>
@@ -6116,7 +6116,7 @@
         <v>-21.476649</v>
       </c>
       <c r="O43" s="45" t="n">
-        <v>-22.0630222741573</v>
+        <v>-22.05831553139014</v>
       </c>
       <c r="P43" s="92" t="n">
         <v>23</v>
@@ -6143,22 +6143,22 @@
       </c>
       <c r="F44" s="91" t="n"/>
       <c r="G44" s="44" t="n">
-        <v>-416.887557</v>
+        <v>-416.995321</v>
       </c>
       <c r="H44" s="42" t="n">
-        <v>-416.460129</v>
+        <v>-416.566972</v>
       </c>
       <c r="I44" s="45" t="n">
-        <v>-416.6944306506024</v>
+        <v>-416.7120059285714</v>
       </c>
       <c r="J44" s="44" t="n">
-        <v>-416.995312</v>
+        <v>-416.995321</v>
       </c>
       <c r="K44" s="42" t="n">
         <v>-416.352375</v>
       </c>
       <c r="L44" s="45" t="n">
-        <v>-416.710499704142</v>
+        <v>-416.7161959230769</v>
       </c>
       <c r="M44" s="44" t="n">
         <v>-417.423726</v>
@@ -6167,7 +6167,7 @@
         <v>-416.352375</v>
       </c>
       <c r="O44" s="45" t="n">
-        <v>-416.9416648207171</v>
+        <v>-416.9403842589641</v>
       </c>
       <c r="P44" s="92" t="n">
         <v>21</v>
@@ -6197,10 +6197,10 @@
         <v>152.461698</v>
       </c>
       <c r="H45" s="42" t="n">
-        <v>152.851823</v>
+        <v>152.851415</v>
       </c>
       <c r="I45" s="45" t="n">
-        <v>152.6691077831325</v>
+        <v>152.6559019880953</v>
       </c>
       <c r="J45" s="44" t="n">
         <v>152.461698</v>
@@ -6209,7 +6209,7 @@
         <v>152.851823</v>
       </c>
       <c r="L45" s="45" t="n">
-        <v>152.6557813668639</v>
+        <v>152.651947112426</v>
       </c>
       <c r="M45" s="44" t="n">
         <v>152.076901</v>
@@ -6218,7 +6218,7 @@
         <v>152.851823</v>
       </c>
       <c r="O45" s="45" t="n">
-        <v>152.4691439482072</v>
+        <v>152.4701706593625</v>
       </c>
       <c r="P45" s="92" t="n">
         <v>25</v>
@@ -6251,7 +6251,7 @@
         <v>-23.723193</v>
       </c>
       <c r="I46" s="45" t="n">
-        <v>-24.10099880722892</v>
+        <v>-24.1012825</v>
       </c>
       <c r="J46" s="44" t="n">
         <v>-24.724972</v>
@@ -6260,7 +6260,7 @@
         <v>-23.723193</v>
       </c>
       <c r="L46" s="45" t="n">
-        <v>-24.25498152071006</v>
+        <v>-24.24905869822485</v>
       </c>
       <c r="M46" s="44" t="n">
         <v>-25.125972</v>
@@ -6269,7 +6269,7 @@
         <v>-23.723193</v>
       </c>
       <c r="O46" s="45" t="n">
-        <v>-24.53610703386454</v>
+        <v>-24.52852592231076</v>
       </c>
       <c r="P46" s="92" t="n">
         <v>4</v>
@@ -6302,7 +6302,7 @@
         <v>-22.384772</v>
       </c>
       <c r="I47" s="45" t="n">
-        <v>-22.66845851807229</v>
+        <v>-22.67594855952381</v>
       </c>
       <c r="J47" s="44" t="n">
         <v>-23.114796</v>
@@ -6311,7 +6311,7 @@
         <v>-22.384772</v>
       </c>
       <c r="L47" s="45" t="n">
-        <v>-22.75569563905325</v>
+        <v>-22.75731213609468</v>
       </c>
       <c r="M47" s="44" t="n">
         <v>-23.388034</v>
@@ -6320,7 +6320,7 @@
         <v>-22.384772</v>
       </c>
       <c r="O47" s="45" t="n">
-        <v>-22.89529466334661</v>
+        <v>-22.89202340438247</v>
       </c>
       <c r="P47" s="92" t="n">
         <v>9</v>
@@ -6353,7 +6353,7 @@
         <v>61.15118</v>
       </c>
       <c r="I48" s="45" t="n">
-        <v>60.81857181012658</v>
+        <v>60.82188389873418</v>
       </c>
       <c r="J48" s="44" t="n">
         <v>60.355442</v>
@@ -6362,7 +6362,7 @@
         <v>61.15118</v>
       </c>
       <c r="L48" s="45" t="n">
-        <v>60.67661245508982</v>
+        <v>60.67848794578313</v>
       </c>
       <c r="M48" s="44" t="n">
         <v>60.092064</v>
@@ -6371,7 +6371,7 @@
         <v>61.15118</v>
       </c>
       <c r="O48" s="45" t="n">
-        <v>60.54909903830645</v>
+        <v>60.55067473790323</v>
       </c>
       <c r="P48" s="92" t="n">
         <v>27</v>
@@ -6404,7 +6404,7 @@
         <v>-67.86762899999999</v>
       </c>
       <c r="I49" s="45" t="n">
-        <v>-68.18770769620254</v>
+        <v>-68.18991998734177</v>
       </c>
       <c r="J49" s="44" t="n">
         <v>-68.74229099999999</v>
@@ -6413,7 +6413,7 @@
         <v>-67.86762899999999</v>
       </c>
       <c r="L49" s="45" t="n">
-        <v>-68.32395424550899</v>
+        <v>-68.32512159638554</v>
       </c>
       <c r="M49" s="44" t="n">
         <v>-68.83043000000001</v>
@@ -6422,7 +6422,7 @@
         <v>-67.86762899999999</v>
       </c>
       <c r="O49" s="45" t="n">
-        <v>-68.3971421391129</v>
+        <v>-68.39731840322581</v>
       </c>
       <c r="P49" s="92" t="n">
         <v>4</v>
@@ -6455,7 +6455,7 @@
         <v>23.356569</v>
       </c>
       <c r="I50" s="45" t="n">
-        <v>23.00539556962025</v>
+        <v>23.00427887341772</v>
       </c>
       <c r="J50" s="44" t="n">
         <v>22.393935</v>
@@ -6464,7 +6464,7 @@
         <v>23.356569</v>
       </c>
       <c r="L50" s="45" t="n">
-        <v>22.82987648502994</v>
+        <v>22.83565985542169</v>
       </c>
       <c r="M50" s="44" t="n">
         <v>21.867993</v>
@@ -6473,7 +6473,7 @@
         <v>23.356569</v>
       </c>
       <c r="O50" s="45" t="n">
-        <v>22.5284381592742</v>
+        <v>22.53602748185484</v>
       </c>
       <c r="P50" s="92" t="n">
         <v>17</v>
@@ -6506,7 +6506,7 @@
         <v>24.679922</v>
       </c>
       <c r="I51" s="45" t="n">
-        <v>24.32429641025641</v>
+        <v>24.32092979012346</v>
       </c>
       <c r="J51" s="44" t="n">
         <v>23.91365</v>
@@ -6515,7 +6515,7 @@
         <v>24.679922</v>
       </c>
       <c r="L51" s="45" t="n">
-        <v>24.25169221153846</v>
+        <v>24.24832285987261</v>
       </c>
       <c r="M51" s="44" t="n">
         <v>23.91365</v>
@@ -6524,7 +6524,7 @@
         <v>24.871068</v>
       </c>
       <c r="O51" s="45" t="n">
-        <v>24.41261841630901</v>
+        <v>24.40745705781585</v>
       </c>
       <c r="P51" s="92" t="n">
         <v>41</v>
@@ -6557,7 +6557,7 @@
         <v>-8.071808000000001</v>
       </c>
       <c r="I52" s="45" t="n">
-        <v>-8.798520493670885</v>
+        <v>-8.810700531645569</v>
       </c>
       <c r="J52" s="44" t="n">
         <v>-9.422999000000001</v>
@@ -6566,7 +6566,7 @@
         <v>-8.071808000000001</v>
       </c>
       <c r="L52" s="45" t="n">
-        <v>-8.9177559</v>
+        <v>-8.919611116959064</v>
       </c>
       <c r="M52" s="44" t="n">
         <v>-9.802823</v>
@@ -6575,7 +6575,7 @@
         <v>-8.071808000000001</v>
       </c>
       <c r="O52" s="45" t="n">
-        <v>-9.140423251497007</v>
+        <v>-9.133573289421157</v>
       </c>
       <c r="P52" s="92" t="n">
         <v>21</v>
@@ -6601,13 +6601,13 @@
       </c>
       <c r="F53" s="91" t="n"/>
       <c r="G53" s="44" t="n">
-        <v>-11.467526</v>
+        <v>-11.467314</v>
       </c>
       <c r="H53" s="42" t="n">
         <v>-10.88194</v>
       </c>
       <c r="I53" s="45" t="n">
-        <v>-11.10391878082192</v>
+        <v>-11.08774624324324</v>
       </c>
       <c r="J53" s="44" t="n">
         <v>-11.467576</v>
@@ -6616,7 +6616,7 @@
         <v>-10.88194</v>
       </c>
       <c r="L53" s="45" t="n">
-        <v>-11.17334998</v>
+        <v>-11.16626253642384</v>
       </c>
       <c r="M53" s="44" t="n">
         <v>-13.421556</v>
@@ -6625,7 +6625,7 @@
         <v>-10.88194</v>
       </c>
       <c r="O53" s="45" t="n">
-        <v>-12.24227311134454</v>
+        <v>-12.22087324</v>
       </c>
       <c r="P53" s="92" t="n">
         <v>35</v>
@@ -6651,13 +6651,13 @@
       </c>
       <c r="F54" s="91" t="n"/>
       <c r="G54" s="44" t="n">
-        <v>40.977668</v>
+        <v>41.525186</v>
       </c>
       <c r="H54" s="42" t="n">
         <v>43.89431</v>
       </c>
       <c r="I54" s="45" t="n">
-        <v>42.68040469863013</v>
+        <v>42.68698493243243</v>
       </c>
       <c r="J54" s="44" t="n">
         <v>40.977668</v>
@@ -6666,7 +6666,7 @@
         <v>43.89431</v>
       </c>
       <c r="L54" s="45" t="n">
-        <v>42.58898082</v>
+        <v>42.57953365562914</v>
       </c>
       <c r="M54" s="44" t="n">
         <v>40.977668</v>
@@ -6675,7 +6675,7 @@
         <v>44.440236</v>
       </c>
       <c r="O54" s="45" t="n">
-        <v>42.86703858403362</v>
+        <v>42.85912994736842</v>
       </c>
       <c r="P54" s="92" t="n">
         <v>45</v>
@@ -6707,7 +6707,7 @@
         <v>-18.859689</v>
       </c>
       <c r="I55" s="45" t="n">
-        <v>-23.02777960714286</v>
+        <v>-22.92665717647059</v>
       </c>
       <c r="J55" s="44" t="n">
         <v>-26.629189</v>
@@ -6716,16 +6716,16 @@
         <v>-18.859689</v>
       </c>
       <c r="L55" s="45" t="n">
-        <v>-23.13839495930232</v>
+        <v>-23.09603113294798</v>
       </c>
       <c r="M55" s="44" t="n">
-        <v>-27.121857</v>
+        <v>-26.629189</v>
       </c>
       <c r="N55" s="42" t="n">
         <v>-18.859689</v>
       </c>
       <c r="O55" s="45" t="n">
-        <v>-23.30883104347826</v>
+        <v>-23.27909397101449</v>
       </c>
       <c r="P55" s="92" t="n">
         <v>10</v>
@@ -6757,7 +6757,7 @@
         <v>837.043891</v>
       </c>
       <c r="I56" s="45" t="n">
-        <v>-1.146315297619048</v>
+        <v>-1.413316776470588</v>
       </c>
       <c r="J56" s="44" t="n">
         <v>-26.18926</v>
@@ -6766,7 +6766,7 @@
         <v>837.043891</v>
       </c>
       <c r="L56" s="45" t="n">
-        <v>18.09662660465116</v>
+        <v>17.85554054913295</v>
       </c>
       <c r="M56" s="44" t="n">
         <v>-26.540071</v>
@@ -6775,7 +6775,7 @@
         <v>841.2395320000001</v>
       </c>
       <c r="O56" s="45" t="n">
-        <v>40.15379519668737</v>
+        <v>38.71268892960663</v>
       </c>
       <c r="P56" s="92" t="n">
         <v>18</v>
@@ -6807,7 +6807,7 @@
         <v>-20.999616</v>
       </c>
       <c r="I57" s="45" t="n">
-        <v>-21.37625388799414</v>
+        <v>-21.37741422165325</v>
       </c>
       <c r="J57" s="44" t="n">
         <v>-21.841877</v>
@@ -6816,7 +6816,7 @@
         <v>-20.999616</v>
       </c>
       <c r="L57" s="45" t="n">
-        <v>-21.4775999836294</v>
+        <v>-21.47716401669565</v>
       </c>
       <c r="M57" s="44" t="n">
         <v>-22.122962</v>
@@ -6825,7 +6825,7 @@
         <v>-20.999616</v>
       </c>
       <c r="O57" s="45" t="n">
-        <v>-21.6350609817066</v>
+        <v>-21.63067301380368</v>
       </c>
       <c r="P57" s="92" t="n">
         <v>26</v>
@@ -6851,13 +6851,13 @@
       </c>
       <c r="F58" s="91" t="n"/>
       <c r="G58" s="44" t="n">
-        <v>-15.890203</v>
+        <v>-15.88976</v>
       </c>
       <c r="H58" s="42" t="n">
         <v>-15.342378</v>
       </c>
       <c r="I58" s="45" t="n">
-        <v>-15.60325250658858</v>
+        <v>-15.58432487710315</v>
       </c>
       <c r="J58" s="44" t="n">
         <v>-16.165521</v>
@@ -6866,7 +6866,7 @@
         <v>-15.342378</v>
       </c>
       <c r="L58" s="45" t="n">
-        <v>-15.76333962312783</v>
+        <v>-15.7436150786087</v>
       </c>
       <c r="M58" s="44" t="n">
         <v>-17.536379</v>
@@ -6875,7 +6875,7 @@
         <v>-15.342378</v>
       </c>
       <c r="O58" s="45" t="n">
-        <v>-16.40963446748495</v>
+        <v>-16.38912216257669</v>
       </c>
       <c r="P58" s="92" t="n">
         <v>22</v>
@@ -6907,7 +6907,7 @@
         <v>-5.590203</v>
       </c>
       <c r="I59" s="45" t="n">
-        <v>-7.167750777777778</v>
+        <v>-7.170056849315069</v>
       </c>
       <c r="J59" s="44" t="n">
         <v>-9.611084</v>
@@ -6916,7 +6916,7 @@
         <v>-5.213486</v>
       </c>
       <c r="L59" s="45" t="n">
-        <v>-7.197122980645161</v>
+        <v>-7.184883832258064</v>
       </c>
       <c r="M59" s="44" t="n">
         <v>-9.802917000000001</v>
@@ -6925,7 +6925,7 @@
         <v>-5.213486</v>
       </c>
       <c r="O59" s="45" t="n">
-        <v>-7.349746347533633</v>
+        <v>-7.336416422818792</v>
       </c>
       <c r="P59" s="92" t="n">
         <v>42.3</v>
@@ -6954,28 +6954,28 @@
         <v>6.214715</v>
       </c>
       <c r="H60" s="42" t="n">
-        <v>14.911674</v>
+        <v>15.699434</v>
       </c>
       <c r="I60" s="45" t="n">
-        <v>10.77423253571428</v>
+        <v>11.30350394047619</v>
       </c>
       <c r="J60" s="44" t="n">
-        <v>-6.661213</v>
+        <v>-5.47143</v>
       </c>
       <c r="K60" s="42" t="n">
-        <v>14.911674</v>
+        <v>15.699434</v>
       </c>
       <c r="L60" s="45" t="n">
-        <v>5.390240947976879</v>
+        <v>6.095987739884393</v>
       </c>
       <c r="M60" s="44" t="n">
         <v>-14.804155</v>
       </c>
       <c r="N60" s="42" t="n">
-        <v>14.911674</v>
+        <v>15.699434</v>
       </c>
       <c r="O60" s="45" t="n">
-        <v>-6.3766511796875</v>
+        <v>-6.038908654296875</v>
       </c>
       <c r="P60" s="92" t="n">
         <v>14</v>
@@ -7004,28 +7004,28 @@
         <v>36.858513</v>
       </c>
       <c r="H61" s="42" t="n">
-        <v>41.50333</v>
+        <v>42.533191</v>
       </c>
       <c r="I61" s="45" t="n">
-        <v>37.9246793974359</v>
+        <v>38.25167724675325</v>
       </c>
       <c r="J61" s="44" t="n">
-        <v>34.40002</v>
+        <v>35.174856</v>
       </c>
       <c r="K61" s="42" t="n">
-        <v>41.50333</v>
+        <v>42.533191</v>
       </c>
       <c r="L61" s="45" t="n">
-        <v>37.14768103508772</v>
+        <v>37.38259697647059</v>
       </c>
       <c r="M61" s="44" t="n">
         <v>33.230358</v>
       </c>
       <c r="N61" s="42" t="n">
-        <v>41.50333</v>
+        <v>42.533191</v>
       </c>
       <c r="O61" s="45" t="n">
-        <v>35.53023926147704</v>
+        <v>35.60057126546906</v>
       </c>
       <c r="P61" s="92" t="n">
         <v>8</v>
@@ -7051,22 +7051,22 @@
       </c>
       <c r="F62" s="91" t="n"/>
       <c r="G62" s="44" t="n">
-        <v>82.615841</v>
+        <v>82.343768</v>
       </c>
       <c r="H62" s="42" t="n">
         <v>83.2949</v>
       </c>
       <c r="I62" s="45" t="n">
-        <v>82.98289884615384</v>
+        <v>82.95056215584415</v>
       </c>
       <c r="J62" s="44" t="n">
-        <v>81.52805600000001</v>
+        <v>81.52930600000001</v>
       </c>
       <c r="K62" s="42" t="n">
         <v>83.2949</v>
       </c>
       <c r="L62" s="45" t="n">
-        <v>82.59979866081872</v>
+        <v>82.63166176470588</v>
       </c>
       <c r="M62" s="44" t="n">
         <v>79.35389600000001</v>
@@ -7075,7 +7075,7 @@
         <v>83.954911</v>
       </c>
       <c r="O62" s="45" t="n">
-        <v>82.54311672654691</v>
+        <v>82.52869057085829</v>
       </c>
       <c r="P62" s="92" t="n">
         <v>16</v>
@@ -7101,31 +7101,31 @@
       </c>
       <c r="F63" s="91" t="n"/>
       <c r="G63" s="44" t="n">
-        <v>-6.509798</v>
+        <v>-5.592806</v>
       </c>
       <c r="H63" s="42" t="n">
-        <v>7.929504</v>
+        <v>10.026499</v>
       </c>
       <c r="I63" s="45" t="n">
-        <v>-0.4139315897435897</v>
+        <v>0.6659212077922078</v>
       </c>
       <c r="J63" s="44" t="n">
-        <v>-13.495672</v>
+        <v>-13.243159</v>
       </c>
       <c r="K63" s="42" t="n">
-        <v>7.929504</v>
+        <v>10.026499</v>
       </c>
       <c r="L63" s="45" t="n">
-        <v>-5.980323286549708</v>
+        <v>-5.270446388235294</v>
       </c>
       <c r="M63" s="44" t="n">
         <v>-26.463295</v>
       </c>
       <c r="N63" s="42" t="n">
-        <v>7.929504</v>
+        <v>10.026499</v>
       </c>
       <c r="O63" s="45" t="n">
-        <v>-16.12693703992016</v>
+        <v>-15.7929541497006</v>
       </c>
       <c r="P63" s="92" t="n">
         <v>1.4</v>
@@ -7157,7 +7157,7 @@
         <v>-85.679993</v>
       </c>
       <c r="I64" s="45" t="n">
-        <v>-86.63040257692307</v>
+        <v>-86.56850481818182</v>
       </c>
       <c r="J64" s="44" t="n">
         <v>-90.739226</v>
@@ -7166,7 +7166,7 @@
         <v>-85.679993</v>
       </c>
       <c r="L64" s="45" t="n">
-        <v>-87.97862091812866</v>
+        <v>-87.8346130117647</v>
       </c>
       <c r="M64" s="44" t="n">
         <v>-101.861621</v>
@@ -7175,7 +7175,7 @@
         <v>-85.679993</v>
       </c>
       <c r="O64" s="45" t="n">
-        <v>-93.33838422155689</v>
+        <v>-93.19901413173653</v>
       </c>
       <c r="P64" s="92" t="n">
         <v>2</v>
@@ -7201,31 +7201,31 @@
       </c>
       <c r="F65" s="91" t="n"/>
       <c r="G65" s="44" t="n">
-        <v>-5.972686</v>
+        <v>-5.972712</v>
       </c>
       <c r="H65" s="42" t="n">
         <v>-5.420091</v>
       </c>
       <c r="I65" s="45" t="n">
-        <v>-5.660575658536586</v>
+        <v>-5.69199831707317</v>
       </c>
       <c r="J65" s="44" t="n">
-        <v>-5.972686</v>
+        <v>-5.972712</v>
       </c>
       <c r="K65" s="42" t="n">
         <v>-4.68231</v>
       </c>
       <c r="L65" s="45" t="n">
-        <v>-5.372702284090909</v>
+        <v>-5.410408238636363</v>
       </c>
       <c r="M65" s="44" t="n">
-        <v>-5.972686</v>
+        <v>-5.972712</v>
       </c>
       <c r="N65" s="42" t="n">
         <v>-2.468425</v>
       </c>
       <c r="O65" s="45" t="n">
-        <v>-4.216228758220502</v>
+        <v>-4.253693208897485</v>
       </c>
       <c r="P65" s="92" t="n">
         <v>8</v>
@@ -7257,7 +7257,7 @@
         <v>15.242623</v>
       </c>
       <c r="I66" s="45" t="n">
-        <v>11.32634341333333</v>
+        <v>11.22494876623377</v>
       </c>
       <c r="J66" s="44" t="n">
         <v>-21.731984</v>
@@ -7266,7 +7266,7 @@
         <v>16.182109</v>
       </c>
       <c r="L66" s="45" t="n">
-        <v>11.05276816049383</v>
+        <v>11.04067568965517</v>
       </c>
       <c r="M66" s="44" t="n">
         <v>-21.731984</v>
@@ -7275,7 +7275,7 @@
         <v>16.182109</v>
       </c>
       <c r="O66" s="45" t="n">
-        <v>11.05276816049383</v>
+        <v>11.04067568965517</v>
       </c>
       <c r="P66" s="92" t="n">
         <v>14</v>
@@ -7307,16 +7307,16 @@
         <v>-3.597945</v>
       </c>
       <c r="I67" s="45" t="n">
-        <v>-3.864065012987013</v>
+        <v>-3.873202730769231</v>
       </c>
       <c r="J67" s="44" t="n">
         <v>-4.323584</v>
       </c>
       <c r="K67" s="42" t="n">
-        <v>-3.580612</v>
+        <v>-3.580661</v>
       </c>
       <c r="L67" s="45" t="n">
-        <v>-3.942969867924528</v>
+        <v>-3.950191666666667</v>
       </c>
       <c r="M67" s="44" t="n">
         <v>-4.831024</v>
@@ -7325,7 +7325,7 @@
         <v>-3.580612</v>
       </c>
       <c r="O67" s="45" t="n">
-        <v>-4.154803769387756</v>
+        <v>-4.149490304081633</v>
       </c>
       <c r="P67" s="92" t="n">
         <v>2</v>
@@ -7354,19 +7354,19 @@
         <v>49.378784</v>
       </c>
       <c r="H68" s="42" t="n">
-        <v>50.323333</v>
+        <v>50.513823</v>
       </c>
       <c r="I68" s="45" t="n">
-        <v>49.82904168333334</v>
+        <v>49.880645984375</v>
       </c>
       <c r="J68" s="44" t="n">
         <v>49.378784</v>
       </c>
       <c r="K68" s="42" t="n">
-        <v>50.323363</v>
+        <v>50.513823</v>
       </c>
       <c r="L68" s="45" t="n">
-        <v>49.88567759859155</v>
+        <v>49.89272302797202</v>
       </c>
       <c r="M68" s="44" t="n">
         <v>49.378784</v>
@@ -7375,7 +7375,7 @@
         <v>51.269342</v>
       </c>
       <c r="O68" s="45" t="n">
-        <v>50.38637744893617</v>
+        <v>50.38061864118896</v>
       </c>
       <c r="P68" s="92" t="n">
         <v>20</v>
@@ -7523,7 +7523,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>